<commit_message>
Code Review 学习 OK
</commit_message>
<xml_diff>
--- a/check-in-record.xlsx
+++ b/check-in-record.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>C、W</t>
   </si>
@@ -1745,7 +1745,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1907,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1919,6 +1919,9 @@
       </c>
       <c r="F8" t="s">
         <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6">

</xml_diff>